<commit_message>
UI updated for manon wedding
</commit_message>
<xml_diff>
--- a/RX10_Settings.xlsx
+++ b/RX10_Settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Sony-A7III-PhotoBooth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D78092-F7A8-4665-8174-F3552B24713C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B6385B-DD6B-4EA3-8B2B-29A75AAD8021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" xr2:uid="{65A07B65-B5FC-4261-8C54-210456D62B36}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>Limite ISO lumière</t>
   </si>
@@ -80,15 +80,6 @@
   </si>
   <si>
     <t>Désactiver le bip</t>
-  </si>
-  <si>
-    <t>Si non branché sur secteur -&gt; Baisser la luminosité de l'écran au minimum</t>
-  </si>
-  <si>
-    <t>Sans doute pas suffisant sur Batterie</t>
-  </si>
-  <si>
-    <t>Voir avec Renata pour récupérer son transfo ou en racheter un</t>
   </si>
   <si>
     <t>Ouverture: f/4 --&gt; f2.4</t>
@@ -942,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1199319A-5879-471D-A7A2-0D0B5D47410A}">
-  <dimension ref="H8:O29"/>
+  <dimension ref="H8:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,12 +1111,12 @@
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="10:10" x14ac:dyDescent="0.25">
@@ -1140,37 +1131,22 @@
     </row>
     <row r="21" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J29" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +1172,7 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6">
@@ -1211,7 +1187,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="7">
@@ -1226,7 +1202,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="8">
@@ -1241,7 +1217,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="D4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -1305,10 +1281,10 @@
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
       <c r="F11" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1319,10 +1295,10 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="D13" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F13" s="13">
         <v>13.2</v>
@@ -1334,10 +1310,10 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F14" s="13">
         <v>8.8000000000000007</v>
@@ -1349,10 +1325,10 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="D15" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F15" s="14">
         <v>1.0999999999999999E-2</v>
@@ -1375,7 +1351,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="15"/>
       <c r="D18" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>5</v>
@@ -1391,10 +1367,10 @@
       <c r="A19" s="3"/>
       <c r="B19" s="15"/>
       <c r="D19" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F19" s="17">
         <v>2.4</v>
@@ -1405,10 +1381,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F20" s="18">
         <f>F18/F13*36</f>
@@ -1431,13 +1407,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F23" s="21">
         <f t="shared" ref="F23:G23" si="4">$C$24*1000</f>
@@ -1450,16 +1426,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C24" s="22">
         <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F24" s="23">
         <f t="shared" ref="F24:G24" si="5">F13</f>
@@ -1478,10 +1454,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D26" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F26" s="7">
         <f t="shared" ref="F26:G26" si="6">F18*(F23/F24+1)/1000</f>
@@ -1494,10 +1470,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D27" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F27" s="25">
         <f t="shared" ref="F27:G27" si="7">F26*1000*F24/F23</f>
@@ -1516,10 +1492,10 @@
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="D29" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F29" s="27">
         <f t="shared" ref="F29:G29" si="8">2*DEGREES(ATAN(F23/2/F26/1000))</f>
@@ -1532,10 +1508,10 @@
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="D30" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F30" s="27">
         <f t="shared" ref="F30:G30" si="9">2*DEGREES(ATAN(F13/(2*F18)))</f>
@@ -1553,13 +1529,13 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
       <c r="E32" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
       <c r="E33" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
@@ -1576,10 +1552,10 @@
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F37" s="24">
         <f t="shared" ref="F37:G37" si="10">(F18^2/(F15*F19)+F18)/1000</f>
@@ -1596,10 +1572,10 @@
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D39" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F39" s="28">
         <f t="shared" ref="F39:G39" si="11">F18/F19</f>
@@ -1618,10 +1594,10 @@
     </row>
     <row r="41" spans="4:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="D41" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F41" s="25">
         <f t="shared" ref="F41:G41" si="12">F27*F39/(F39-F15)</f>
@@ -1634,10 +1610,10 @@
     </row>
     <row r="42" spans="4:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="D42" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F42" s="25">
         <f t="shared" ref="F42:G42" si="13">F39*F27/(F39+F15)</f>
@@ -1650,10 +1626,10 @@
     </row>
     <row r="43" spans="4:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="D43" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F43" s="21">
         <f t="shared" ref="F43:G43" si="14">F$18*F41/(F41-F$18)</f>
@@ -1666,10 +1642,10 @@
     </row>
     <row r="44" spans="4:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="D44" s="29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F44" s="21">
         <f t="shared" ref="F44:G44" si="15">IF(F42&lt;=F18,"∞",F$18*F42/(F42-F$18))</f>
@@ -1682,10 +1658,10 @@
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D45" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F45" s="30">
         <f t="shared" ref="F45:G45" si="16">IF(F42&lt;=F18,"∞",F44-F43)</f>

</xml_diff>